<commit_message>
Beginning the process of manually assembing the CO2 flux files. Done DOY 179, 182, 183, 192, 195, 196.
</commit_message>
<xml_diff>
--- a/data/Data_Information.xlsx
+++ b/data/Data_Information.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/declantaylor/Documents/Work/Henry_Lab/Alex2022/honours_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5718141-7C3E-8844-9EA3-D430ED95372F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9D43F-2FBF-0D48-8FB4-249F916C467F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{E7395AF2-8F4A-6C49-BDF4-16D2DC2507BE}"/>
   </bookViews>
   <sheets>
     <sheet name="IRGA_flux" sheetId="1" r:id="rId1"/>
+    <sheet name="Soil Moisture" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Due to frequent and evolving challenges with the data logger equipment, we have significant amounts of incomplete IRGA flux data.</t>
   </si>
@@ -63,6 +64,63 @@
   </si>
   <si>
     <t>IRGA recorded 12C, 14C, 13C, 11C. The end of 11C and all of the T plots were done by video. The IRGA .DAT file was manually combined with my created CSV.</t>
+  </si>
+  <si>
+    <t>DRYAS</t>
+  </si>
+  <si>
+    <t>DRYAS_002 (from 1103 to 1147) is merely a subset of DRYAS_001 (1043 to 1147). Captures all but T11 and C12.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ASSEMBLED</t>
+  </si>
+  <si>
+    <t>MEAD</t>
+  </si>
+  <si>
+    <t>Manual collection.</t>
+  </si>
+  <si>
+    <t>IRGA FLUX DATA</t>
+  </si>
+  <si>
+    <t>NEXT STEPS</t>
+  </si>
+  <si>
+    <t>13 and 14 plots were done in the morning (when 11 and 12 data was erased), 11 and 12 were recorded in the afternoon.</t>
+  </si>
+  <si>
+    <t>Sucessful IRGA data recording</t>
+  </si>
+  <si>
+    <t>PERIOD</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>A note about delayed fans and other such notes: I start the 2min from when the fans were turned on, not before.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>close?</t>
+  </si>
+  <si>
+    <t>Soil Moisture</t>
+  </si>
+  <si>
+    <t>We have lots of sets of "full SM days" and then extra SM measurements at CO2 plots on days we measured CO2.</t>
+  </si>
+  <si>
+    <t>In all cases, we have now-averaged SM values per plot, in long-data across all sites, stamped with DOY.</t>
+  </si>
+  <si>
+    <t>Found in "2022_SM_ALLSITES.csv".</t>
   </si>
 </sst>
 </file>
@@ -423,50 +481,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA02A40-213D-8A4E-A457-5B46C7C06A2C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>179</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>182</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>183</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>192</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>195</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>196</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>197</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>206</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>207</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>208</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A41751-6D4A-7D44-9F24-C70B3DDDECB3}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>179</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>